<commit_message>
added grades of lesson 8
</commit_message>
<xml_diff>
--- a/chartgrades.xlsx
+++ b/chartgrades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sarah's files\جيل الأمل\صيف 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sarah's files\جيل الأمل\صيف 2020\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E6B50C-FD15-464F-8598-EFE4E232C16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B09D61B-B83D-42A4-B666-07119276E676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{62361AB2-85DC-4D95-B398-2C00A771B72B}"/>
   </bookViews>
@@ -311,19 +311,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>20</c:v>
@@ -332,7 +332,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10</c:v>
@@ -341,7 +341,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5</c:v>
@@ -1707,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA65AE7-791B-41D4-AEED-40BCA9060FA0}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1870,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -1892,7 +1892,7 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>30</v>
@@ -1903,7 +1903,7 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -1914,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -1947,7 +1947,7 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -1980,7 +1980,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>10</v>

</xml_diff>

<commit_message>
added grades of lsn 9
</commit_message>
<xml_diff>
--- a/chartgrades.xlsx
+++ b/chartgrades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sarah's files\جيل الأمل\صيف 2020\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B09D61B-B83D-42A4-B666-07119276E676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C921ECB3-1F11-4B64-8BB8-1C068AF81F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{62361AB2-85DC-4D95-B398-2C00A771B72B}"/>
   </bookViews>
@@ -311,19 +311,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>20</c:v>
@@ -332,7 +332,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10</c:v>
@@ -341,7 +341,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5</c:v>
@@ -515,19 +515,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -536,7 +536,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1707,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA65AE7-791B-41D4-AEED-40BCA9060FA0}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1870,10 +1870,10 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C16">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1892,10 +1892,10 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1903,10 +1903,10 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1914,10 +1914,10 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1947,10 +1947,10 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1980,7 +1980,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>10</v>

</xml_diff>

<commit_message>
lsn 10 summary + lsn 10 grades + updated grades image for last two lsns
</commit_message>
<xml_diff>
--- a/chartgrades.xlsx
+++ b/chartgrades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sarah's files\جيل الأمل\صيف 2020\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C921ECB3-1F11-4B64-8BB8-1C068AF81F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50DE0D6-1FD4-4E34-B2B0-E4D227360601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{62361AB2-85DC-4D95-B398-2C00A771B72B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>التكليف</t>
   </si>
@@ -70,12 +70,6 @@
   </si>
   <si>
     <t>فاروق</t>
-  </si>
-  <si>
-    <t>محمود</t>
-  </si>
-  <si>
-    <t>الاسم</t>
   </si>
 </sst>
 </file>
@@ -262,9 +256,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$16:$A$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$16:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>أحمد ملبنجي</c:v>
                 </c:pt>
@@ -297,42 +298,46 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>فاروق</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>محمود</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$27</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$16:$B$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$16:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10</c:v>
@@ -341,10 +346,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,9 +468,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$16:$A$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$16:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>أحمد ملبنجي</c:v>
                 </c:pt>
@@ -501,27 +510,31 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>فاروق</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>محمود</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$27</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$16:$C$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$16:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15</c:v>
@@ -536,7 +549,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -546,9 +559,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA65AE7-791B-41D4-AEED-40BCA9060FA0}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A15:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1717,146 +1727,6 @@
     <col min="3" max="3" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>1</v>
@@ -1870,10 +1740,10 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1881,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1892,10 +1762,10 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1903,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -1914,7 +1784,7 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>25</v>
@@ -1925,7 +1795,7 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1947,10 +1817,10 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C23">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1980,21 +1850,10 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>